<commit_message>
Added second delivery files
</commit_message>
<xml_diff>
--- a/Artifacts/Individual Contribution Metrics.xlsx
+++ b/Artifacts/Individual Contribution Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnosuady-my.sharepoint.com/personal/a15004035_alumnos_uady_mx/Documents/Sexto Semestre/HCI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Github\HCI2021\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3CEE575-62DA-455F-AC49-7913C427686A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C94AB7-0B35-4440-B69F-894A24D58C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{682EC480-9E5D-43F8-B6D4-011330CF2DD8}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12204" xr2:uid="{682EC480-9E5D-43F8-B6D4-011330CF2DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -97,8 +97,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,11 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +457,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,15 +521,15 @@
       </c>
       <c r="I3">
         <f>SUM(E2:E25)</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="J3">
         <f>SUM(F2:F25)</f>
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="K3">
         <f>SUM(G2:G25)</f>
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -544,15 +553,15 @@
       </c>
       <c r="I4">
         <f>(I3/(SUM(I3:K3)))*100</f>
-        <v>30.434782608695656</v>
+        <v>35</v>
       </c>
       <c r="J4">
         <f>(J3/(SUM(I3:K3)))*100</f>
-        <v>34.782608695652172</v>
+        <v>32.5</v>
       </c>
       <c r="K4">
         <f>(K3/(SUM(I3:K3)))*100</f>
-        <v>34.782608695652172</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -585,6 +594,9 @@
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
       <c r="F6">
         <v>5</v>
       </c>
@@ -600,6 +612,15 @@
         <v>7</v>
       </c>
       <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
     </row>
@@ -624,6 +645,15 @@
       <c r="C9">
         <v>13</v>
       </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -635,6 +665,15 @@
       <c r="C10">
         <v>5</v>
       </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -668,6 +707,7 @@
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -675,5 +715,6 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated individual contribution metrics
</commit_message>
<xml_diff>
--- a/Artifacts/Individual Contribution Metrics.xlsx
+++ b/Artifacts/Individual Contribution Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Github\HCI2021\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C94AB7-0B35-4440-B69F-894A24D58C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921C104-41F3-4A26-9B0F-92E37BAA7929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12204" xr2:uid="{682EC480-9E5D-43F8-B6D4-011330CF2DD8}"/>
+    <workbookView xWindow="4032" yWindow="2460" windowWidth="21600" windowHeight="11328" xr2:uid="{682EC480-9E5D-43F8-B6D4-011330CF2DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>Total Points</t>
+  </si>
+  <si>
+    <t>Usability Tests</t>
+  </si>
+  <si>
+    <t>Final interfaces</t>
+  </si>
+  <si>
+    <t>HCI Article</t>
+  </si>
+  <si>
+    <t>HCI Poster</t>
+  </si>
+  <si>
+    <t>HCI Video</t>
+  </si>
+  <si>
+    <t>Usability Test Artifacts (script, checklist)</t>
   </si>
 </sst>
 </file>
@@ -136,10 +154,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EAE09C-CB1E-4DF7-BE30-59403C09907A}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,16 +484,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -521,15 +539,15 @@
       </c>
       <c r="I3">
         <f>SUM(E2:E25)</f>
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="J3">
         <f>SUM(F2:F25)</f>
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="K3">
         <f>SUM(G2:G25)</f>
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -553,15 +571,15 @@
       </c>
       <c r="I4">
         <f>(I3/(SUM(I3:K3)))*100</f>
-        <v>35</v>
+        <v>35.37117903930131</v>
       </c>
       <c r="J4">
         <f>(J3/(SUM(I3:K3)))*100</f>
-        <v>32.5</v>
+        <v>36.244541484716159</v>
       </c>
       <c r="K4">
         <f>(K3/(SUM(I3:K3)))*100</f>
-        <v>32.5</v>
+        <v>28.384279475982531</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -634,6 +652,12 @@
       <c r="C8">
         <v>5</v>
       </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -685,6 +709,15 @@
       <c r="C11">
         <v>8</v>
       </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -696,6 +729,9 @@
       <c r="C12">
         <v>2</v>
       </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -707,7 +743,115 @@
       <c r="C13">
         <v>5</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update Individual Contribution Metrics.xlsx
</commit_message>
<xml_diff>
--- a/Artifacts/Individual Contribution Metrics.xlsx
+++ b/Artifacts/Individual Contribution Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Github\HCI2021\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921C104-41F3-4A26-9B0F-92E37BAA7929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC4F261-BFE6-46AD-BA43-943FDAB2FDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4032" yWindow="2460" windowWidth="21600" windowHeight="11328" xr2:uid="{682EC480-9E5D-43F8-B6D4-011330CF2DD8}"/>
   </bookViews>
@@ -152,12 +152,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EAE09C-CB1E-4DF7-BE30-59403C09907A}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,7 +540,7 @@
       </c>
       <c r="I3">
         <f>SUM(E2:E25)</f>
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J3">
         <f>SUM(F2:F25)</f>
@@ -571,15 +572,15 @@
       </c>
       <c r="I4">
         <f>(I3/(SUM(I3:K3)))*100</f>
-        <v>35.37117903930131</v>
+        <v>37.552742616033754</v>
       </c>
       <c r="J4">
         <f>(J3/(SUM(I3:K3)))*100</f>
-        <v>36.244541484716159</v>
+        <v>35.021097046413502</v>
       </c>
       <c r="K4">
         <f>(K3/(SUM(I3:K3)))*100</f>
-        <v>28.384279475982531</v>
+        <v>27.426160337552741</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -809,6 +810,9 @@
       <c r="C17">
         <v>8</v>
       </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
       <c r="F17">
         <v>8</v>
       </c>
@@ -849,7 +853,7 @@
       <c r="F19">
         <v>5</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>